<commit_message>
Avance del sistema - Modulo Reportes | Detalles
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -214,7 +214,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -224,13 +224,28 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -245,8 +260,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,19 +567,23 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="95.405" bestFit="true" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>